<commit_message>
Change name to businesses
</commit_message>
<xml_diff>
--- a/Data/19_dataText/dataText.xlsx
+++ b/Data/19_dataText/dataText.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/19_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="8_{1D01AD94-356A-411C-8978-8CB75BD80CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4375798D-6816-4A4C-B773-F1E618FA5DF4}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{1D01AD94-356A-411C-8978-8CB75BD80CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E90560BE-31B5-4AEB-A9B2-AF975AAD86FD}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -131,9 +131,6 @@
 Achievements are the number of learners who successfully complete an individual aim in an academic year.</t>
   </si>
   <si>
-    <t>An enterprise can be thought of as the overall business, made up of all the individual sites or workplaces.</t>
-  </si>
-  <si>
     <t>This data is experimental. ONS are continuing to develop these statistics and aim to move to SOC profession grouping and publish data regularly. The timescale for the next release has not yet been agreed.</t>
   </si>
   <si>
@@ -216,6 +213,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Represented here are enterprises, which can be thought of as the overall business, made up of all the individual sites or workplaces.</t>
   </si>
 </sst>
 </file>
@@ -598,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C14" sqref="C12:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -627,13 +627,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="58">
@@ -641,13 +641,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="58">
@@ -655,13 +655,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="58">
@@ -669,13 +669,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="116">
@@ -683,13 +683,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="58">
@@ -697,13 +697,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="58">
@@ -711,13 +711,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="58">
@@ -725,13 +725,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="87">
@@ -739,13 +739,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -753,7 +753,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="58">
@@ -761,13 +761,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="130.5">
@@ -775,13 +775,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="130.5">
@@ -789,13 +789,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="203">
@@ -803,13 +803,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="203">
@@ -817,13 +817,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="203">
@@ -831,13 +831,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="203">
@@ -845,13 +845,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="203">
@@ -859,13 +859,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="203">
@@ -873,13 +873,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="116">
@@ -887,13 +887,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="154.5">
@@ -901,13 +901,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="154.5">
@@ -915,13 +915,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix load errors fix white space in buckinghamshire add lsip lat and long fix data text metric names tidycode
</commit_message>
<xml_diff>
--- a/Data/19_dataText/dataText.xlsx
+++ b/Data/19_dataText/dataText.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/19_dataText/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\19_dataText\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{7D9602D3-E8FE-4498-9EE9-995C8A24B656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD02C53A-B63A-49E7-8C66-BA2E05049117}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3231EB7-7141-4564-A3BC-635B4E7EDB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -53,15 +53,6 @@
     <t>Employment</t>
   </si>
   <si>
-    <t xml:space="preserve">  Self Employed </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Unemployed </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Inactive </t>
-  </si>
-  <si>
     <t>vacancies</t>
   </si>
   <si>
@@ -273,6 +264,15 @@
   </si>
   <si>
     <t>AY20/21</t>
+  </si>
+  <si>
+    <t>SelfEmployed</t>
+  </si>
+  <si>
+    <t>Unemployed</t>
+  </si>
+  <si>
+    <t>Inactive</t>
   </si>
 </sst>
 </file>
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -675,22 +675,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="58">
@@ -698,19 +698,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="58">
@@ -718,19 +718,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="58">
@@ -738,19 +738,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="58">
@@ -758,19 +758,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="116">
@@ -778,350 +778,350 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="58">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="58">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="58">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="87">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="58">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="130.5">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="130.5">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="203">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="203">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="203">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="203">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="203">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="203">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="116">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="154.5">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="154.5">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clarify naming of per 100k rates
</commit_message>
<xml_diff>
--- a/Data/19_dataText/dataText.xlsx
+++ b/Data/19_dataText/dataText.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/hannah_cox_education_gov_uk/Documents/Documents/Projects/lsip_dashboard/Data/19_dataText/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\19_dataText\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{B3231EB7-7141-4564-A3BC-635B4E7EDB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDB8E2B4-2D6D-47D6-9B6F-02A8A903BA1A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59ACB7BD-699D-40A8-BF6D-2286FC87EA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
   <sheets>
     <sheet name="dataText" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="70">
   <si>
     <t>empRate</t>
   </si>
@@ -258,10 +258,6 @@
     <t xml:space="preserve">  Inactive </t>
   </si>
   <si>
-    <t xml:space="preserve">Further education and skills include all age apprenticeships and publicly-funded adult (19+) learning, including community learning, delivered by an FE institution, a training provider or within a local community. 
-Rates are per 100,000 people. </t>
-  </si>
-  <si>
     <t>Further education and skills include all age apprenticeships and publicly-funded adult (19+) learning, including community learning, delivered by an FE institution, a training provider or within a local community. 
 Rates are per 100,000 people</t>
   </si>
@@ -292,6 +288,14 @@
 A sustained apprenticeship is recorded when 6 months continuous participation is recorded at any point in the destination year (between August 2020 and July 2021).
 Not recorded includes pupils who were captured in the destination source data but who failed to meet the sustained participation criteria.
 Unknown (activity not captured): The student was not found to have any participation in education, apprenticeship or employment nor recorded as receiving out-of-work benefits at any point in the year. This also includes not being recorded by their Local Authority as NEET (not engaged in education, employment or training).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The rates are the number of achievments in AY21/22 per 100,000 of the population. Further education and skills include all age apprenticeships and publicly-funded adult (19+) learning, including community learning, delivered by an FE institution, a training provider or within a local community. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The rates are the number of participants in AY21/22 per 100,000 of the population. Further education and skills include all age apprenticeships and publicly-funded adult (19+) learning, including community learning, delivered by an FE institution, a training provider or within a local community. 
+</t>
   </si>
 </sst>
 </file>
@@ -688,15 +692,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="8.73046875" style="6"/>
-    <col min="5" max="5" width="57.265625" customWidth="1"/>
-    <col min="6" max="6" width="113.46484375" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="6"/>
+    <col min="5" max="5" width="57.26953125" customWidth="1"/>
+    <col min="6" max="6" width="113.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -719,7 +723,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="57">
+    <row r="2" spans="1:6" ht="58">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -739,7 +743,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="57">
+    <row r="3" spans="1:6" ht="58">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -759,7 +763,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="57">
+    <row r="4" spans="1:6" ht="58">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -779,7 +783,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="57">
+    <row r="5" spans="1:6" ht="58">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -799,7 +803,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="114">
+    <row r="6" spans="1:6" ht="116">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -819,7 +823,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="57">
+    <row r="7" spans="1:6" ht="58">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -839,7 +843,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="57">
+    <row r="8" spans="1:6" ht="58">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -859,7 +863,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="57">
+    <row r="9" spans="1:6" ht="58">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -879,7 +883,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="85.5">
+    <row r="10" spans="1:6" ht="87">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -910,7 +914,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="57">
+    <row r="12" spans="1:6" ht="58">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -930,7 +934,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="128.25">
+    <row r="13" spans="1:6" ht="130.5">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -950,7 +954,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="128.25">
+    <row r="14" spans="1:6" ht="130.5">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -978,7 +982,7 @@
         <v>55</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
         <v>26</v>
@@ -998,7 +1002,7 @@
         <v>55</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D16" t="s">
         <v>26</v>
@@ -1018,7 +1022,7 @@
         <v>55</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" t="s">
         <v>26</v>
@@ -1030,7 +1034,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="199.5">
+    <row r="18" spans="1:6" ht="203">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1038,7 +1042,7 @@
         <v>55</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
         <v>26</v>
@@ -1050,7 +1054,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="199.5">
+    <row r="19" spans="1:6" ht="203">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1058,7 +1062,7 @@
         <v>55</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
         <v>26</v>
@@ -1070,7 +1074,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="199.5">
+    <row r="20" spans="1:6" ht="203">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1078,7 +1082,7 @@
         <v>55</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D20" t="s">
         <v>26</v>
@@ -1090,7 +1094,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="114">
+    <row r="21" spans="1:6" ht="116">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1118,13 +1122,13 @@
         <v>57</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>39</v>
@@ -1138,13 +1142,13 @@
         <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
added all of harris text based changes
</commit_message>
<xml_diff>
--- a/Data/19_dataText/dataText.xlsx
+++ b/Data/19_dataText/dataText.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\19_dataText\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59ACB7BD-699D-40A8-BF6D-2286FC87EA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA724CDF-21CD-4875-82BB-DDBFAEFF6B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="176">
   <si>
     <t>empRate</t>
   </si>
@@ -249,15 +249,6 @@
     <t>AY20/21</t>
   </si>
   <si>
-    <t xml:space="preserve">  Self Employed </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Unemployed </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Inactive </t>
-  </si>
-  <si>
     <t>Further education and skills include all age apprenticeships and publicly-funded adult (19+) learning, including community learning, delivered by an FE institution, a training provider or within a local community. 
 Rates are per 100,000 people</t>
   </si>
@@ -297,12 +288,339 @@
     <t xml:space="preserve">The rates are the number of participants in AY21/22 per 100,000 of the population. Further education and skills include all age apprenticeships and publicly-funded adult (19+) learning, including community learning, delivered by an FE institution, a training provider or within a local community. 
 </t>
   </si>
+  <si>
+    <t>The employment rate</t>
+  </si>
+  <si>
+    <t>The self-employment rate</t>
+  </si>
+  <si>
+    <t>The unemployment rate</t>
+  </si>
+  <si>
+    <t>The inactivity rate</t>
+  </si>
+  <si>
+    <t>Self-employment</t>
+  </si>
+  <si>
+    <t>Unemployment</t>
+  </si>
+  <si>
+    <t>Inactivity</t>
+  </si>
+  <si>
+    <t>The number of online job adverts</t>
+  </si>
+  <si>
+    <t>The number of businesses</t>
+  </si>
+  <si>
+    <t>Business birth rates</t>
+  </si>
+  <si>
+    <t>Business death rates</t>
+  </si>
+  <si>
+    <t>FE achievements in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FE participation </t>
+  </si>
+  <si>
+    <t>The FE achievement rate per 100,000</t>
+  </si>
+  <si>
+    <t>The FE participation rate per 100,000</t>
+  </si>
+  <si>
+    <t>The proportion of people qualified at Level 3 or above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sustained positive destination rate after study at Key Stage 4 in </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sustained positive destination rate after study at Key Stage 5 in </t>
+  </si>
+  <si>
+    <t>mapComment</t>
+  </si>
+  <si>
+    <t>SelfEmployed</t>
+  </si>
+  <si>
+    <t>Unemployed</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>employment rates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The employment rate in </t>
+  </si>
+  <si>
+    <t>Employment rate</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employment rates are </t>
+  </si>
+  <si>
+    <t>self-employment rates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The self-employment rate in </t>
+  </si>
+  <si>
+    <t>Self-employment rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Self-employment rates are </t>
+  </si>
+  <si>
+    <t>unemployment rates</t>
+  </si>
+  <si>
+    <t>Unemployment rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unemployment rates are </t>
+  </si>
+  <si>
+    <t>inactivity rates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The inactivity rate in </t>
+  </si>
+  <si>
+    <t>Inactivity rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inactivity rates are </t>
+  </si>
+  <si>
+    <t>employment volumes</t>
+  </si>
+  <si>
+    <t>Employment in</t>
+  </si>
+  <si>
+    <t>employment volume</t>
+  </si>
+  <si>
+    <t>Employment is</t>
+  </si>
+  <si>
+    <t>self-employment volumes</t>
+  </si>
+  <si>
+    <t>Self-employment in</t>
+  </si>
+  <si>
+    <t>self-employment volume</t>
+  </si>
+  <si>
+    <t>Self-employment is</t>
+  </si>
+  <si>
+    <t>unemployment volumes</t>
+  </si>
+  <si>
+    <t>Unemployment in</t>
+  </si>
+  <si>
+    <t>unemployment volume</t>
+  </si>
+  <si>
+    <t>Unemployment is</t>
+  </si>
+  <si>
+    <t>inactivity volumes</t>
+  </si>
+  <si>
+    <t>Inactivity in</t>
+  </si>
+  <si>
+    <t>inactivity volume</t>
+  </si>
+  <si>
+    <t>Inactivity is</t>
+  </si>
+  <si>
+    <t>online job adverts</t>
+  </si>
+  <si>
+    <t>Online job adverts</t>
+  </si>
+  <si>
+    <t>number of online job adverts</t>
+  </si>
+  <si>
+    <t>The number of online job adverts is</t>
+  </si>
+  <si>
+    <t>the number of businesses</t>
+  </si>
+  <si>
+    <t>The number of businesses in</t>
+  </si>
+  <si>
+    <t>Businesses</t>
+  </si>
+  <si>
+    <t>number of businesses</t>
+  </si>
+  <si>
+    <t>The number of businesses is</t>
+  </si>
+  <si>
+    <t>business birth rates</t>
+  </si>
+  <si>
+    <t>The business birth rate in</t>
+  </si>
+  <si>
+    <t>Business birth rate</t>
+  </si>
+  <si>
+    <t>business birth rate</t>
+  </si>
+  <si>
+    <t>Business birth rates are</t>
+  </si>
+  <si>
+    <t>business death rates</t>
+  </si>
+  <si>
+    <t>The business death rate in</t>
+  </si>
+  <si>
+    <t>Business death rate</t>
+  </si>
+  <si>
+    <t>business death rate</t>
+  </si>
+  <si>
+    <t>Business death rates are</t>
+  </si>
+  <si>
+    <t>FE achievement volumes</t>
+  </si>
+  <si>
+    <t>The number of FE achievements</t>
+  </si>
+  <si>
+    <t>FE achievements</t>
+  </si>
+  <si>
+    <t>The FE achievements</t>
+  </si>
+  <si>
+    <t>number of FE achievements</t>
+  </si>
+  <si>
+    <t>FE achievements are</t>
+  </si>
+  <si>
+    <t>FE participation volumes</t>
+  </si>
+  <si>
+    <t>FE participation</t>
+  </si>
+  <si>
+    <t>FE participation volume</t>
+  </si>
+  <si>
+    <t>FE participation is</t>
+  </si>
+  <si>
+    <t>FE achievement rates per 100,000</t>
+  </si>
+  <si>
+    <t>FE achievement rate per 100,000</t>
+  </si>
+  <si>
+    <t>The FE achievement rate per 100,000 is</t>
+  </si>
+  <si>
+    <t>FE participation rates per 100,000</t>
+  </si>
+  <si>
+    <t>FE participation rate per 100,000</t>
+  </si>
+  <si>
+    <t>The FE participation rate per 100,000 is</t>
+  </si>
+  <si>
+    <t>the proportions of people qualified at Level 3 or above</t>
+  </si>
+  <si>
+    <t>Qualified at Level 3 or above</t>
+  </si>
+  <si>
+    <t>proportion of people qualified at Level 3 or above</t>
+  </si>
+  <si>
+    <t>The proportion of people qualified at Level 3 or above is</t>
+  </si>
+  <si>
+    <t>key stage 4 sustained positive destination rates</t>
+  </si>
+  <si>
+    <t>Key stage 4 sustained positive destination rate</t>
+  </si>
+  <si>
+    <t>key stage 4 destinations</t>
+  </si>
+  <si>
+    <t>key stage 4 sustained positive destination rate</t>
+  </si>
+  <si>
+    <t>The sustained positive destination rate after study at Key Stage 4 is</t>
+  </si>
+  <si>
+    <t>key stage 5 sustained positive destination rates</t>
+  </si>
+  <si>
+    <t>Key stage 5 sustained positive destination rate</t>
+  </si>
+  <si>
+    <t>key stage 5 destinations</t>
+  </si>
+  <si>
+    <t>key stage 5 sustained positive destination rate</t>
+  </si>
+  <si>
+    <t>The sustained positive destination rate after study at Key Stage 5 is</t>
+  </si>
+  <si>
+    <t>timeTitle</t>
+  </si>
+  <si>
+    <t>timeComment</t>
+  </si>
+  <si>
+    <t>mapPop</t>
+  </si>
+  <si>
+    <t>breakdownTitle</t>
+  </si>
+  <si>
+    <t>breakdownComment</t>
+  </si>
+  <si>
+    <t>LaComment</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,6 +658,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -349,7 +672,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -357,11 +680,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -376,6 +714,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,20 +1031,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="8.7265625" style="6"/>
-    <col min="5" max="5" width="57.26953125" customWidth="1"/>
-    <col min="6" max="6" width="113.453125" customWidth="1"/>
+    <col min="5" max="5" width="32.08984375" customWidth="1"/>
+    <col min="6" max="6" width="51.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:13" ht="15" thickBot="1">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -722,8 +1063,29 @@
       <c r="F1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="58">
+      <c r="G1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I1" t="s">
+        <v>171</v>
+      </c>
+      <c r="J1" t="s">
+        <v>172</v>
+      </c>
+      <c r="K1" t="s">
+        <v>173</v>
+      </c>
+      <c r="L1" t="s">
+        <v>174</v>
+      </c>
+      <c r="M1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="73" thickBot="1">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -742,8 +1104,29 @@
       <c r="F2" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="58">
+      <c r="G2" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="73" thickBot="1">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -762,8 +1145,29 @@
       <c r="F3" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="58">
+      <c r="G3" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="73" thickBot="1">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -782,8 +1186,29 @@
       <c r="F4" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="58">
+      <c r="G4" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="73" thickBot="1">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -802,8 +1227,29 @@
       <c r="F5" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="116">
+      <c r="G5" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="174.5" thickBot="1">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -822,10 +1268,31 @@
       <c r="F6" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="58">
+      <c r="G6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="73" thickBot="1">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>49</v>
@@ -842,10 +1309,31 @@
       <c r="F7" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="58">
+      <c r="G7" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="73" thickBot="1">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>50</v>
@@ -862,10 +1350,31 @@
       <c r="F8" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="58">
+      <c r="G8" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="73" thickBot="1">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>51</v>
@@ -882,8 +1391,29 @@
       <c r="F9" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="87">
+      <c r="G9" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="145.5" thickBot="1">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -902,41 +1432,113 @@
       <c r="F10" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="87.5" thickBot="1">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="58">
+        <v>41</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="261.5" thickBot="1">
       <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="130.5">
+        <v>36</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="261.5" thickBot="1">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>54</v>
@@ -953,36 +1555,78 @@
       <c r="F13" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="130.5">
+      <c r="G13" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="363" thickBot="1">
       <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>41</v>
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="409.5">
+        <v>37</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="363" thickBot="1">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>68</v>
+      <c r="C15" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="D15" t="s">
         <v>26</v>
@@ -993,16 +1637,37 @@
       <c r="F15" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="409.5">
+      <c r="G15" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="409.6" thickBot="1">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D16" t="s">
         <v>26</v>
@@ -1013,16 +1678,37 @@
       <c r="F16" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="409.5">
+      <c r="G16" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="409.6" thickBot="1">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D17" t="s">
         <v>26</v>
@@ -1033,126 +1719,204 @@
       <c r="F17" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="203">
+      <c r="G17" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="203.5" thickBot="1">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="263" thickBot="1">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="203">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="7" t="s">
+      <c r="F19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="254" thickBot="1">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
         <v>63</v>
       </c>
-      <c r="D19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="203">
-      <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>23</v>
+      <c r="D20" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="116">
+        <v>39</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15" thickBot="1">
       <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="E21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="154.5">
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:13" ht="409.6" thickBot="1">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>65</v>
+        <v>55</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="145.5">
+        <v>37</v>
+      </c>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:13" ht="363" thickBot="1">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>39</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="G23" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
fix a drag down year error change a few names
</commit_message>
<xml_diff>
--- a/Data/19_dataText/dataText.xlsx
+++ b/Data/19_dataText/dataText.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\19_dataText\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA724CDF-21CD-4875-82BB-DDBFAEFF6B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55532DF-1DCA-4BDC-93C2-A4B78AD0C889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="169">
   <si>
     <t>empRate</t>
   </si>
@@ -210,34 +210,10 @@
     <t>Oct-Sep 2022</t>
   </si>
   <si>
-    <t>Oct-Sep 2023</t>
-  </si>
-  <si>
-    <t>Oct-Sep 2024</t>
-  </si>
-  <si>
-    <t>Oct-Sep 2025</t>
-  </si>
-  <si>
-    <t>Oct-Sep 2026</t>
-  </si>
-  <si>
-    <t>Oct-Sep 2027</t>
-  </si>
-  <si>
-    <t>Oct-Sep 2028</t>
-  </si>
-  <si>
-    <t>Oct-Sep 2029</t>
-  </si>
-  <si>
     <t>Dec 2022</t>
   </si>
   <si>
     <t>Mar 2022</t>
-  </si>
-  <si>
-    <t>Dec 2020 - Dec 2021 (</t>
   </si>
   <si>
     <t>AY21/22</t>
@@ -614,6 +590,9 @@
   </si>
   <si>
     <t>LaComment</t>
+  </si>
+  <si>
+    <t>Dec 2020 - Dec 2021</t>
   </si>
 </sst>
 </file>
@@ -1033,13 +1012,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="8.7265625" style="6"/>
+    <col min="2" max="2" width="25" style="6" customWidth="1"/>
     <col min="5" max="5" width="32.08984375" customWidth="1"/>
     <col min="6" max="6" width="51.26953125" customWidth="1"/>
   </cols>
@@ -1064,25 +1043,25 @@
         <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H1" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="I1" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="J1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="K1" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="L1" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="M1" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="73" thickBot="1">
@@ -1105,25 +1084,25 @@
         <v>32</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="73" thickBot="1">
@@ -1131,7 +1110,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>40</v>
@@ -1146,25 +1125,25 @@
         <v>32</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="73" thickBot="1">
@@ -1172,7 +1151,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>40</v>
@@ -1187,25 +1166,25 @@
         <v>32</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="I4" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="J4" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>98</v>
-      </c>
       <c r="L4" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="M4" s="8" t="s">
         <v>92</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="73" thickBot="1">
@@ -1213,7 +1192,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>40</v>
@@ -1228,25 +1207,25 @@
         <v>32</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="174.5" thickBot="1">
@@ -1254,7 +1233,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>40</v>
@@ -1272,30 +1251,30 @@
         <v>4</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="73" thickBot="1">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>40</v>
@@ -1310,33 +1289,33 @@
         <v>32</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="73" thickBot="1">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>40</v>
@@ -1351,33 +1330,33 @@
         <v>32</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="73" thickBot="1">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>40</v>
@@ -1392,25 +1371,25 @@
         <v>32</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="145.5" thickBot="1">
@@ -1418,7 +1397,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>24</v>
@@ -1433,25 +1412,25 @@
         <v>34</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="87.5" thickBot="1">
@@ -1459,7 +1438,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>41</v>
@@ -1474,25 +1453,25 @@
         <v>35</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="261.5" thickBot="1">
@@ -1500,7 +1479,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>54</v>
+        <v>168</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>41</v>
@@ -1515,25 +1494,25 @@
         <v>36</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="261.5" thickBot="1">
@@ -1541,7 +1520,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>168</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>41</v>
@@ -1556,25 +1535,25 @@
         <v>36</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="363" thickBot="1">
@@ -1582,10 +1561,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
         <v>26</v>
@@ -1597,25 +1576,25 @@
         <v>37</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="363" thickBot="1">
@@ -1623,10 +1602,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
         <v>26</v>
@@ -1638,25 +1617,25 @@
         <v>37</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="409.6" thickBot="1">
@@ -1664,10 +1643,10 @@
         <v>10</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D16" t="s">
         <v>26</v>
@@ -1679,25 +1658,25 @@
         <v>37</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="409.6" thickBot="1">
@@ -1705,10 +1684,10 @@
         <v>11</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
         <v>26</v>
@@ -1720,25 +1699,25 @@
         <v>37</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="203.5" thickBot="1">
@@ -1746,7 +1725,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>40</v>
@@ -1761,25 +1740,25 @@
         <v>38</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="263" thickBot="1">
@@ -1787,40 +1766,40 @@
         <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>39</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="254" thickBot="1">
@@ -1828,40 +1807,40 @@
         <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>39</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15" thickBot="1">
@@ -1881,10 +1860,10 @@
         <v>12</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D22" t="s">
         <v>26</v>
@@ -1902,10 +1881,10 @@
         <v>15</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D23" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
change sto code to getthe working futures data into the dashboard ignored all the data files as they are not public
</commit_message>
<xml_diff>
--- a/Data/19_dataText/dataText.xlsx
+++ b/Data/19_dataText/dataText.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\19_dataText\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55532DF-1DCA-4BDC-93C2-A4B78AD0C889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991F491A-C201-44B2-BFC8-F2770D808600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="177">
   <si>
     <t>empRate</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>vacancies</t>
-  </si>
-  <si>
-    <t>workingFutures</t>
   </si>
   <si>
     <t>enterpriseCount</t>
@@ -593,6 +590,33 @@
   </si>
   <si>
     <t>Dec 2020 - Dec 2021</t>
+  </si>
+  <si>
+    <t>wfEmployment</t>
+  </si>
+  <si>
+    <t>2035</t>
+  </si>
+  <si>
+    <t>To come</t>
+  </si>
+  <si>
+    <t>Forecasted employment</t>
+  </si>
+  <si>
+    <t>forecasted employment volumes</t>
+  </si>
+  <si>
+    <t>forecasted employment volume</t>
+  </si>
+  <si>
+    <t>Forecasted employment is</t>
+  </si>
+  <si>
+    <t>forecasted employment volume growth</t>
+  </si>
+  <si>
+    <t>Forecasted employment growth in</t>
   </si>
 </sst>
 </file>
@@ -1012,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1025,43 +1049,43 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
-        <v>22</v>
-      </c>
       <c r="G1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I1" t="s">
         <v>162</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>163</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>164</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>165</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>166</v>
-      </c>
-      <c r="M1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="73" thickBot="1">
@@ -1069,40 +1093,40 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="L2" s="8" t="s">
+      <c r="M2" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="73" thickBot="1">
@@ -1110,40 +1134,40 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H3" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="M3" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="73" thickBot="1">
@@ -1151,40 +1175,40 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="J4" s="8" t="s">
+      <c r="K4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="M4" s="8" t="s">
         <v>91</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="73" thickBot="1">
@@ -1192,40 +1216,40 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="J5" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="K5" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="M5" s="8" t="s">
         <v>95</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="174.5" thickBot="1">
@@ -1233,163 +1257,163 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="H6" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>97</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>98</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L6" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="M6" s="8" t="s">
         <v>99</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="73" thickBot="1">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H7" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="J7" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="L7" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="L7" s="8" t="s">
+      <c r="M7" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="73" thickBot="1">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H8" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="J8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="L8" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="J8" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="L8" s="8" t="s">
+      <c r="M8" s="8" t="s">
         <v>107</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="73" thickBot="1">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H9" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="J9" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="L9" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="J9" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="L9" s="8" t="s">
+      <c r="M9" s="8" t="s">
         <v>111</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="145.5" thickBot="1">
@@ -1397,503 +1421,532 @@
         <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H10" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="J10" s="8" t="s">
+      <c r="K10" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="L10" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="L10" s="8" t="s">
+      <c r="M10" s="8" t="s">
         <v>115</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="87.5" thickBot="1">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H11" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="J11" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="K11" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="L11" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="L11" s="8" t="s">
+      <c r="M11" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="261.5" thickBot="1">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H12" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="I12" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="J12" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="K12" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="L12" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="L12" s="8" t="s">
+      <c r="M12" s="8" t="s">
         <v>125</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="261.5" thickBot="1">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H13" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="I13" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="J13" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="K13" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="L13" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="K13" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="L13" s="8" t="s">
+      <c r="M13" s="8" t="s">
         <v>130</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="363" thickBot="1">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H14" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="J14" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="K14" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="L14" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="M14" s="8" t="s">
         <v>136</v>
-      </c>
-      <c r="M14" s="8" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="363" thickBot="1">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H15" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="J15" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="L15" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="J15" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="L15" s="8" t="s">
+      <c r="M15" s="8" t="s">
         <v>140</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="409.6" thickBot="1">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H16" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="J16" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="I16" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="J16" s="8" t="s">
+      <c r="K16" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="M16" s="8" t="s">
         <v>143</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="M16" s="8" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="409.6" thickBot="1">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H17" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J17" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="I17" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="J17" s="8" t="s">
+      <c r="K17" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="M17" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="M17" s="8" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="203.5" thickBot="1">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H18" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="J18" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="I18" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="J18" s="8" t="s">
+      <c r="K18" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="L18" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="K18" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="L18" s="8" t="s">
+      <c r="M18" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="M18" s="8" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="263" thickBot="1">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H19" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="J19" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="I19" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="J19" s="8" t="s">
+      <c r="K19" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="L19" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="L19" s="8" t="s">
+      <c r="M19" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="254" thickBot="1">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="F20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H20" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="J20" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="I20" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="J20" s="8" t="s">
+      <c r="K20" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="L20" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="L20" s="8" t="s">
+      <c r="M20" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="M20" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="15" thickBot="1">
+    </row>
+    <row r="21" spans="1:13" ht="42.5" thickBot="1">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>168</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>169</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>40</v>
+        <v>170</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>170</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G21" s="8"/>
+        <v>170</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="M21" s="8" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="22" spans="1:13" ht="409.6" thickBot="1">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:13" ht="363" thickBot="1">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G23" s="8"/>
     </row>

</xml_diff>

<commit_message>
made all the snetences kind of make sense
</commit_message>
<xml_diff>
--- a/Data/19_dataText/dataText.xlsx
+++ b/Data/19_dataText/dataText.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\19_dataText\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991F491A-C201-44B2-BFC8-F2770D808600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F00BB6-0173-45C8-BE3A-0B8B767B173F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="193">
   <si>
     <t>empRate</t>
   </si>
@@ -204,24 +204,6 @@
     <t>LatestPeriod</t>
   </si>
   <si>
-    <t>Oct-Sep 2022</t>
-  </si>
-  <si>
-    <t>Dec 2022</t>
-  </si>
-  <si>
-    <t>Mar 2022</t>
-  </si>
-  <si>
-    <t>AY21/22</t>
-  </si>
-  <si>
-    <t>2021</t>
-  </si>
-  <si>
-    <t>AY20/21</t>
-  </si>
-  <si>
     <t>Further education and skills include all age apprenticeships and publicly-funded adult (19+) learning, including community learning, delivered by an FE institution, a training provider or within a local community. 
 Rates are per 100,000 people</t>
   </si>
@@ -481,9 +463,6 @@
     <t>Business death rates are</t>
   </si>
   <si>
-    <t>FE achievement volumes</t>
-  </si>
-  <si>
     <t>The number of FE achievements</t>
   </si>
   <si>
@@ -541,9 +520,6 @@
     <t>The proportion of people qualified at Level 3 or above is</t>
   </si>
   <si>
-    <t>key stage 4 sustained positive destination rates</t>
-  </si>
-  <si>
     <t>Key stage 4 sustained positive destination rate</t>
   </si>
   <si>
@@ -556,9 +532,6 @@
     <t>The sustained positive destination rate after study at Key Stage 4 is</t>
   </si>
   <si>
-    <t>key stage 5 sustained positive destination rates</t>
-  </si>
-  <si>
     <t>Key stage 5 sustained positive destination rate</t>
   </si>
   <si>
@@ -589,34 +562,114 @@
     <t>LaComment</t>
   </si>
   <si>
-    <t>Dec 2020 - Dec 2021</t>
-  </si>
-  <si>
     <t>wfEmployment</t>
   </si>
   <si>
-    <t>2035</t>
-  </si>
-  <si>
     <t>To come</t>
   </si>
   <si>
-    <t>Forecasted employment</t>
-  </si>
-  <si>
-    <t>forecasted employment volumes</t>
-  </si>
-  <si>
-    <t>forecasted employment volume</t>
-  </si>
-  <si>
-    <t>Forecasted employment is</t>
-  </si>
-  <si>
-    <t>forecasted employment volume growth</t>
-  </si>
-  <si>
-    <t>Forecasted employment growth in</t>
+    <t>Growth from 2023 to 2035</t>
+  </si>
+  <si>
+    <t>Oct-Sep 2022 data</t>
+  </si>
+  <si>
+    <t>Dec 2022 data</t>
+  </si>
+  <si>
+    <t>Mar 2022 data</t>
+  </si>
+  <si>
+    <t>Dec 2020 - Dec 2021 data</t>
+  </si>
+  <si>
+    <t>AY21/22 data</t>
+  </si>
+  <si>
+    <t>2021 data</t>
+  </si>
+  <si>
+    <t>AY20/21 data</t>
+  </si>
+  <si>
+    <t>Projected employment growth</t>
+  </si>
+  <si>
+    <t>Projected employment growth from 2023 to 2035</t>
+  </si>
+  <si>
+    <t>projected employment volume changes</t>
+  </si>
+  <si>
+    <t>projected employment volume change</t>
+  </si>
+  <si>
+    <t>are employment rates changing</t>
+  </si>
+  <si>
+    <t>are self-employment rates changing</t>
+  </si>
+  <si>
+    <t>are unemployment rates changing</t>
+  </si>
+  <si>
+    <t>are inactivity rates changing</t>
+  </si>
+  <si>
+    <t>are employment volumes changing</t>
+  </si>
+  <si>
+    <t>are self-employment volumes changing</t>
+  </si>
+  <si>
+    <t>are unemployment volumes changing</t>
+  </si>
+  <si>
+    <t>are inactivity volumes changing</t>
+  </si>
+  <si>
+    <t>are online job adverts changing</t>
+  </si>
+  <si>
+    <t>are the number of businesses changing</t>
+  </si>
+  <si>
+    <t>are business birth rates changing</t>
+  </si>
+  <si>
+    <t>are business death rates changing</t>
+  </si>
+  <si>
+    <t>are FE achievement volumes changing</t>
+  </si>
+  <si>
+    <t>are FE participation volumes changing</t>
+  </si>
+  <si>
+    <t>are FE achievement rates per 100,000 changing</t>
+  </si>
+  <si>
+    <t>are FE participation rates per 100,000 changing</t>
+  </si>
+  <si>
+    <t>are the proportions of people qualified at Level 3 or above changing</t>
+  </si>
+  <si>
+    <t>are key stage 4 sustained positive destination rates changing</t>
+  </si>
+  <si>
+    <t>are key stage 5 sustained positive destination rates changing</t>
+  </si>
+  <si>
+    <t>will year on year employment volume growth change</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;
+  &lt;li&gt;The projections presented in this Workbook are calculated from a number of different data sources, using a variety of econometric and statistical techniques. As a result, precise margins of error cannot be assigned to the estimates. For further details, see the Working Futures Technical Report. &lt;/li&gt;
+ &lt;li&gt;Industries are based on SIC 2007 codes. &lt;/li&gt;
+ &lt;li&gt;Time series of the breakdowns can be downloaded in the data download section or in the publication. &lt;/li&gt;
+ &lt;li&gt;Further breakdowns are available in the published data eg gender, full-time/part-time, as well combined breakdowns. Replacement demand is also available. &lt;/li&gt;
+&lt;/ol&gt;</t>
   </si>
 </sst>
 </file>
@@ -1036,8 +1089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1067,25 +1120,25 @@
         <v>21</v>
       </c>
       <c r="G1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="H1" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="I1" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="J1" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="K1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="L1" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="M1" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="73" thickBot="1">
@@ -1093,7 +1146,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>43</v>
+        <v>161</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>39</v>
@@ -1108,25 +1161,25 @@
         <v>31</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>80</v>
+        <v>172</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="73" thickBot="1">
@@ -1134,7 +1187,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>43</v>
+        <v>161</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>39</v>
@@ -1149,25 +1202,25 @@
         <v>31</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>85</v>
+        <v>173</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="73" thickBot="1">
@@ -1175,7 +1228,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>43</v>
+        <v>161</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>39</v>
@@ -1190,25 +1243,25 @@
         <v>31</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>89</v>
+        <v>174</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="73" thickBot="1">
@@ -1216,7 +1269,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>43</v>
+        <v>161</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>39</v>
@@ -1231,25 +1284,25 @@
         <v>31</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="174.5" thickBot="1">
@@ -1257,7 +1310,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>43</v>
+        <v>161</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>39</v>
@@ -1275,30 +1328,30 @@
         <v>4</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>96</v>
+        <v>176</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="73" thickBot="1">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>43</v>
+        <v>161</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>39</v>
@@ -1313,33 +1366,33 @@
         <v>31</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>100</v>
+        <v>177</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="73" thickBot="1">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>43</v>
+        <v>161</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>39</v>
@@ -1354,33 +1407,33 @@
         <v>31</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>104</v>
+        <v>178</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="73" thickBot="1">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>43</v>
+        <v>161</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>39</v>
@@ -1395,25 +1448,25 @@
         <v>31</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>108</v>
+        <v>179</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="145.5" thickBot="1">
@@ -1421,7 +1474,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>44</v>
+        <v>162</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>23</v>
@@ -1436,25 +1489,25 @@
         <v>33</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>112</v>
+        <v>180</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="87.5" thickBot="1">
@@ -1462,7 +1515,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>45</v>
+        <v>163</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>40</v>
@@ -1477,25 +1530,25 @@
         <v>34</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>116</v>
+        <v>181</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="261.5" thickBot="1">
@@ -1503,7 +1556,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>40</v>
@@ -1518,25 +1571,25 @@
         <v>35</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>121</v>
+        <v>182</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="261.5" thickBot="1">
@@ -1544,7 +1597,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>40</v>
@@ -1559,25 +1612,25 @@
         <v>35</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>126</v>
+        <v>183</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="363" thickBot="1">
@@ -1585,10 +1638,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>46</v>
+        <v>165</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
         <v>25</v>
@@ -1600,25 +1653,25 @@
         <v>36</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>131</v>
+        <v>184</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="363" thickBot="1">
@@ -1626,10 +1679,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>46</v>
+        <v>165</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D15" t="s">
         <v>25</v>
@@ -1641,25 +1694,25 @@
         <v>36</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>137</v>
+        <v>185</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="409.6" thickBot="1">
@@ -1667,10 +1720,10 @@
         <v>9</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>46</v>
+        <v>165</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
         <v>25</v>
@@ -1682,25 +1735,25 @@
         <v>36</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>141</v>
+        <v>186</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="409.6" thickBot="1">
@@ -1708,10 +1761,10 @@
         <v>10</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>46</v>
+        <v>165</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
         <v>25</v>
@@ -1723,25 +1776,25 @@
         <v>36</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>144</v>
+        <v>187</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="203.5" thickBot="1">
@@ -1749,7 +1802,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>47</v>
+        <v>166</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>39</v>
@@ -1764,25 +1817,25 @@
         <v>37</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>147</v>
+        <v>188</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="263" thickBot="1">
@@ -1790,40 +1843,40 @@
         <v>16</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>48</v>
+        <v>167</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>29</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>38</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="254" thickBot="1">
@@ -1831,92 +1884,90 @@
         <v>17</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C20" t="s">
         <v>48</v>
-      </c>
-      <c r="C20" t="s">
-        <v>54</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>38</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>156</v>
+        <v>190</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="K20" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="203.5" thickBot="1">
+      <c r="A21" t="s">
         <v>158</v>
       </c>
-      <c r="L20" s="8" t="s">
+      <c r="B21" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="M20" s="8" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="42.5" thickBot="1">
-      <c r="A21" t="s">
+      <c r="D21" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="G21" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="H21" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J21" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="K21" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="G21" s="8" t="s">
+      <c r="L21" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="H21" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="M21" s="8" t="s">
-        <v>174</v>
-      </c>
+      <c r="M21" s="8"/>
     </row>
     <row r="22" spans="1:13" ht="409.6" thickBot="1">
       <c r="A22" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>46</v>
+        <v>165</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
         <v>25</v>
@@ -1934,10 +1985,10 @@
         <v>14</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>46</v>
+        <v>165</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
added in data caveats for aps data and a generalpoint about misinterpretation. added link for skills imperative data
</commit_message>
<xml_diff>
--- a/Data/19_dataText/dataText.xlsx
+++ b/Data/19_dataText/dataText.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\19_dataText\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92251E1-3FF4-4299-9CB7-E5F2BC3F2278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8F94EE-762E-4092-B055-3B62BE3D8236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="dataText" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -135,63 +136,6 @@
     <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/1703fe2c-2e57-4bfe-9325-08db08498a11'&gt;National Pupil Database&lt;/a&gt;</t>
   </si>
   <si>
-    <t>&lt;ol&gt;
-  &lt;li&gt;Figures are for 16-64 year olds.&lt;/li&gt;
-&lt;li&gt;Years represent Oct to Sep period. So 2017 is the Oct 2017 – Sep 2018 period.&lt;/li&gt;
-&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ol&gt;
-  &lt;li&gt;Employment volumes are for 16-64 year olds.&lt;/li&gt;
-&lt;li&gt;Industry split volumes are for all ages. &lt;/li&gt;
-&lt;li&gt;Years represent Oct to Sep period. So 2017 is the Oct 2017 – Sep 2018 period.&lt;/li&gt;
-&lt;li&gt;Standard Occupational Classification 2010 (SOC2010). The ONS have announced that, due to a coding error, their occupational data should be used with caution. For more information see the data tab.&lt;/li&gt;
-&lt;li&gt;Industry groups are Standard Industrial Classification: SIC 2007.&lt;/li&gt;
-&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ol&gt;
-  &lt;li&gt;These statistics should be treated as experimental, as they are still subject to testing the ability to meet user needs.&lt;/li&gt;
-&lt;li&gt;Duplication of adverts can occur when the same job is posted on multiple job boards, or when multiple recruiters advertise the job at the same time.&lt;/li&gt;
-&lt;li&gt;Counts have been rounded to the nearest 5. Totals may not add due to this rounding.&lt;/li&gt;
-&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ol&gt;
-  &lt;li&gt;Overall total may not equal the sum of all industries due to rounding and suppression.&lt;/li&gt;
- &lt;li&gt;Unregistered businesses that are not large enough to be registered for VAT or PAYE are not included.&lt;/li&gt;
-&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ol&gt;
-  &lt;li&gt;A birth is identified as a business that was present in year t, but did not exist in year t-1 or t-2. Births are identified by making comparison of annual active population files and identifying those present in the latest file, but not the two previous ones.&lt;/li&gt;
- &lt;li&gt;A death is defined as a business that was on the active file in year t, but was no longer present in the active file in t+1 and t+2. In order to provide an early estimate of deaths, an adjustment has been made to the latest two years deaths to allow for reactivations. These figures are provisional and subject to revision.&lt;/li&gt;
- &lt;li&gt;An IDBR birth does not always represent the start of trading, as some businesses register for VAT or PAYE many years into their existence. And businesses that die on IDBR can continue trading if the death has been triggered by a VAT deregistration.&lt;/li&gt;
-&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ol&gt;
-  &lt;li&gt;Total achievements is the count of learners that completed their qualification at any point during the stated academic period.&lt;/li&gt;
- &lt;li&gt;Learners achieving more than one course will appear only once in the grand total.&lt;/li&gt;
- &lt;li&gt;Years shown represent academic years.&lt;/li&gt;
-&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ol&gt;
-  &lt;li&gt;Figures are for 16-64 year olds.&lt;/li&gt;
- &lt;li&gt;NVQ3 or above consists of NVQ3 and NVQ4. &lt;/li&gt;
- &lt;li&gt;NVQ3: 2+ A Levels/VCEs, 4+ AS Levels, Higher School Certificate, Progression/Advanced Diploma, Welsh Baccalaureate Advanced Diploma, NVQ Level 3; Advanced GNVQ, City and Guilds Advanced Craft, ONC, OND, BTEC National, RSA Advanced Diploma.&lt;/li&gt;
- &lt;li&gt;NVQ4 or above: Degree (for example BA, BSc), Higher Degree (for example MA, PhD, PGCE), NVQ Level 4-5, HNC, HND, RSA Higher Diploma, BTEC Higher level, Foundation degree (NI), Professional qualifications (for example teaching, nursing, accountancy).&lt;/li&gt;
-&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ol&gt;
-  &lt;li&gt;Data based on destinations of state-funded mainstream schools.&lt;/li&gt;
- &lt;li&gt;There is no double counting across destinations, a young person is reported in one destination category only.&lt;/li&gt;
- &lt;li&gt;If a student is registered as being in education and an apprenticeship, it is recorded as a sustained education and if a student is registered in employment along with an apprenticeship or in education, it is recorded as sustained employment.&lt;/li&gt;
-&lt;/ol&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -671,11 +615,78 @@
   </si>
   <si>
     <t>&lt;ol&gt;
-  &lt;li&gt;The projections presented in this Workbook are calculated from a number of different data sources, using a variety of econometric and statistical techniques. As a result, precise margins of error cannot be assigned to the estimates. For further details, see the Working Futures Technical Report. &lt;/li&gt;
+  &lt;li&gt;Figures are for 16-64 year olds.&lt;/li&gt;
+&lt;li&gt;Each estimate from the Annual Population Survey carries a margin of error. These are available in the original data via NOMIS. Large margins of error are usually associated with groups with only a small number of respondents. Therefore, please take caution when interpreting data from small subgroups.&lt;/li&gt;
+&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;
+  &lt;li&gt;Employment volumes are for 16-64 year olds.&lt;/li&gt;
+&lt;li&gt;Industry split volumes are for all ages. &lt;/li&gt;
+&lt;li&gt;Each estimate from the Annual Population Survey carries a margin of error. These are available in the original data via NOMIS. Large margins of error are usually associated with groups with only a small number of respondents. Therefore, please take caution when interpreting data from small subgroups.&lt;/li&gt;
+&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
+&lt;li&gt;Standard Occupational Classification 2010 (SOC2010). The ONS have announced that, due to a coding error, their occupational data should be used with caution. For more information see the data tab.&lt;/li&gt;
+&lt;li&gt;Industry groups are Standard Industrial Classification: SIC 2007.&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;
+  &lt;li&gt;These statistics should be treated as experimental, as they are still subject to testing the ability to meet user needs.&lt;/li&gt;
+&lt;li&gt;Duplication of adverts can occur when the same job is posted on multiple job boards, or when multiple recruiters advertise the job at the same time.&lt;/li&gt;
+&lt;li&gt;Counts have been rounded to the nearest 5. Totals may not add due to this rounding.&lt;/li&gt;
+&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;
+  &lt;li&gt;Overall total may not equal the sum of all industries due to rounding and suppression.&lt;/li&gt;
+ &lt;li&gt;Unregistered businesses that are not large enough to be registered for VAT or PAYE are not included.&lt;/li&gt;
+&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;
+  &lt;li&gt;A birth is identified as a business that was present in year t, but did not exist in year t-1 or t-2. Births are identified by making comparison of annual active population files and identifying those present in the latest file, but not the two previous ones.&lt;/li&gt;
+ &lt;li&gt;A death is defined as a business that was on the active file in year t, but was no longer present in the active file in t+1 and t+2. In order to provide an early estimate of deaths, an adjustment has been made to the latest two years deaths to allow for reactivations. These figures are provisional and subject to revision.&lt;/li&gt;
+ &lt;li&gt;An IDBR birth does not always represent the start of trading, as some businesses register for VAT or PAYE many years into their existence. And businesses that die on IDBR can continue trading if the death has been triggered by a VAT deregistration.&lt;/li&gt;
+&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;
+  &lt;li&gt;Total achievements is the count of learners that completed their qualification at any point during the stated academic period.&lt;/li&gt;
+ &lt;li&gt;Learners achieving more than one course will appear only once in the grand total.&lt;/li&gt;
+ &lt;li&gt;Years shown represent academic years.&lt;/li&gt;
+&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;
+  &lt;li&gt;Figures are for 16-64 year olds.&lt;/li&gt;
+&lt;li&gt;Each estimate from the Annual Population Survey carries a margin of error. These are available in the original data via NOMIS. Large margins of error are usually associated with groups with only a small number of respondents. Therefore, please take caution when interpreting data from small subgroups.&lt;/li&gt;
+&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
+ &lt;li&gt;NVQ3 or above consists of NVQ3 and NVQ4. &lt;/li&gt;
+ &lt;li&gt;NVQ3: 2+ A Levels/VCEs, 4+ AS Levels, Higher School Certificate, Progression/Advanced Diploma, Welsh Baccalaureate Advanced Diploma, NVQ Level 3; Advanced GNVQ, City and Guilds Advanced Craft, ONC, OND, BTEC National, RSA Advanced Diploma.&lt;/li&gt;
+ &lt;li&gt;NVQ4 or above: Degree (for example BA, BSc), Higher Degree (for example MA, PhD, PGCE), NVQ Level 4-5, HNC, HND, RSA Higher Diploma, BTEC Higher level, Foundation degree (NI), Professional qualifications (for example teaching, nursing, accountancy).&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;
+  &lt;li&gt;Data based on destinations of state-funded mainstream schools.&lt;/li&gt;
+ &lt;li&gt;There is no double counting across destinations, a young person is reported in one destination category only.&lt;/li&gt;
+ &lt;li&gt;If a student is registered as being in education and an apprenticeship, it is recorded as a sustained education and if a student is registered in employment along with an apprenticeship or in education, it is recorded as sustained employment.&lt;/li&gt;
+&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;
+  &lt;li&gt;The projections presented in this Workbook are calculated from a number of different data sources, using a variety of econometric and statistical techniques. As a result, precise margins of error cannot be assigned to the estimates. For further details, see the Technical Report. &lt;/li&gt;
  &lt;li&gt;Industries are based on SIC 2007 codes. &lt;/li&gt;
  &lt;li&gt;Time series of the breakdowns can be downloaded in the data download section or in the publication. &lt;/li&gt;
  &lt;li&gt;Further breakdowns are available in the published data eg gender, full-time/part-time, as well combined breakdowns. Replacement demand is also available. &lt;/li&gt;
  &lt;li&gt;The projections were largely prepared before the Russian invasion of Ukraine, its subsequent economic effects and policy responses to these events. These factors will have a significant impact on the short-term prospects for the British economy and labour market &lt;/li&gt;
+&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
 &lt;/ol&gt;</t>
   </si>
 </sst>
@@ -1096,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1112,10 +1123,10 @@
         <v>18</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
         <v>19</v>
@@ -1127,361 +1138,361 @@
         <v>21</v>
       </c>
       <c r="G1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="I1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="J1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="K1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="L1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="M1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="73" thickBot="1">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="189" thickBot="1">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>31</v>
+        <v>186</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="73" thickBot="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="189" thickBot="1">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>31</v>
+        <v>186</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="73" thickBot="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="189" thickBot="1">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>31</v>
+        <v>186</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="I4" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="J4" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>83</v>
-      </c>
       <c r="L4" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="M4" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="M4" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="73" thickBot="1">
+    </row>
+    <row r="5" spans="1:13" ht="189" thickBot="1">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>31</v>
+        <v>186</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="174.5" thickBot="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="290.5" thickBot="1">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>32</v>
+        <v>187</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="73" thickBot="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="189" thickBot="1">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="189" thickBot="1">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="73" thickBot="1">
-      <c r="A8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="189" thickBot="1">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="73" thickBot="1">
-      <c r="A9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>31</v>
+        <v>186</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="145.5" thickBot="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="203.5" thickBot="1">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>23</v>
@@ -1493,151 +1504,151 @@
         <v>23</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>33</v>
+        <v>188</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="87.5" thickBot="1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="145.5" thickBot="1">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>34</v>
+        <v>189</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="261.5" thickBot="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="319.5" thickBot="1">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>35</v>
+        <v>190</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="261.5" thickBot="1">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="319.5" thickBot="1">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>35</v>
+        <v>190</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="363" thickBot="1">
@@ -1645,10 +1656,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
         <v>25</v>
@@ -1657,28 +1668,28 @@
         <v>22</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>36</v>
+        <v>191</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="363" thickBot="1">
@@ -1686,10 +1697,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
         <v>25</v>
@@ -1698,28 +1709,28 @@
         <v>22</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>36</v>
+        <v>191</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="409.6" thickBot="1">
@@ -1727,10 +1738,10 @@
         <v>9</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
         <v>25</v>
@@ -1739,28 +1750,28 @@
         <v>22</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>36</v>
+        <v>191</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="409.6" thickBot="1">
@@ -1768,10 +1779,10 @@
         <v>10</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
         <v>25</v>
@@ -1780,69 +1791,69 @@
         <v>22</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>36</v>
+        <v>191</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="203.5" thickBot="1">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="348.5" thickBot="1">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>37</v>
+        <v>192</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="263" thickBot="1">
@@ -1850,40 +1861,40 @@
         <v>16</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>29</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>38</v>
+        <v>193</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="254" thickBot="1">
@@ -1891,78 +1902,78 @@
         <v>17</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>38</v>
+        <v>193</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="L20" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="334" thickBot="1">
+      <c r="A21" t="s">
         <v>150</v>
       </c>
-      <c r="M20" s="8" t="s">
+      <c r="B21" s="6" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="276" thickBot="1">
-      <c r="A21" t="s">
-        <v>158</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>159</v>
-      </c>
       <c r="C21" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="E21" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>194</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="M21" s="8"/>
     </row>
@@ -1971,10 +1982,10 @@
         <v>11</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D22" t="s">
         <v>25</v>
@@ -1983,7 +1994,7 @@
         <v>22</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>36</v>
+        <v>191</v>
       </c>
       <c r="G22" s="8"/>
     </row>
@@ -1992,10 +2003,10 @@
         <v>14</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -2004,7 +2015,7 @@
         <v>22</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>36</v>
+        <v>191</v>
       </c>
       <c r="G23" s="8"/>
     </row>

</xml_diff>

<commit_message>
Fix a few problems with NOMIS formating where we deleted hyphens out of names Fix a few problems with jpb adverts using old LA names Deleted a few unused files
</commit_message>
<xml_diff>
--- a/Data/19_dataText/dataText.xlsx
+++ b/Data/19_dataText/dataText.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\19_dataText\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27D1717-65AD-4B5C-AA8C-2BAABF20A1D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC324C14-B6B2-44DE-9418-F7510B056E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="195">
-  <si>
-    <t>empRate</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="196">
   <si>
     <t>selfempRate</t>
   </si>
@@ -687,6 +684,12 @@
   </si>
   <si>
     <t>&lt;a href = 'https://www.gov.uk/government/publications/labour-market-and-skills-projections-2020-to-2035'&gt;Skills Imperative 2035&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>inemploymentRate</t>
+  </si>
+  <si>
+    <t>inemployment</t>
   </si>
 </sst>
 </file>
@@ -1106,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1119,902 +1122,902 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
       <c r="G1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I1" t="s">
         <v>144</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>145</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>146</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>147</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>148</v>
-      </c>
-      <c r="M1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="189" thickBot="1">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>194</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I2" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="L2" s="8" t="s">
+      <c r="M2" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="189" thickBot="1">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="M3" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="189" thickBot="1">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J4" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="M4" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="189" thickBot="1">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I5" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="J5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="K5" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="M5" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="290.5" thickBot="1">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>195</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I6" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="L6" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="J6" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="L6" s="8" t="s">
+      <c r="M6" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="189" thickBot="1">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I7" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="L7" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="L7" s="8" t="s">
+      <c r="M7" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="189" thickBot="1">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I8" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="L8" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="J8" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="L8" s="8" t="s">
+      <c r="M8" s="8" t="s">
         <v>92</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="189" thickBot="1">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I9" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="L9" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="J9" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="L9" s="8" t="s">
+      <c r="M9" s="8" t="s">
         <v>96</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="203.5" thickBot="1">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J10" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="L10" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="K10" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="L10" s="8" t="s">
+      <c r="M10" s="8" t="s">
         <v>100</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="145.5" thickBot="1">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I11" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="J11" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="K11" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="L11" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="K11" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="L11" s="8" t="s">
+      <c r="M11" s="8" t="s">
         <v>105</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="319.5" thickBot="1">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I12" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="J12" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="K12" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="L12" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="K12" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="L12" s="8" t="s">
+      <c r="M12" s="8" t="s">
         <v>110</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="319.5" thickBot="1">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I13" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="J13" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="K13" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="L13" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="K13" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="L13" s="8" t="s">
+      <c r="M13" s="8" t="s">
         <v>115</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="363" thickBot="1">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I14" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="J14" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="K14" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="L14" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="M14" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="M14" s="8" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="363" thickBot="1">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I15" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="L15" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="J15" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="L15" s="8" t="s">
+      <c r="M15" s="8" t="s">
         <v>124</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="409.6" thickBot="1">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J16" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="M16" s="8" t="s">
         <v>127</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="M16" s="8" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="409.6" thickBot="1">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J17" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="M17" s="8" t="s">
         <v>130</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="M17" s="8" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="348.5" thickBot="1">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J18" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="L18" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="K18" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="L18" s="8" t="s">
+      <c r="M18" s="8" t="s">
         <v>134</v>
-      </c>
-      <c r="M18" s="8" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="263" thickBot="1">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J19" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="K19" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="L19" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="L19" s="8" t="s">
+      <c r="M19" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="254" thickBot="1">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="F20" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J20" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="K20" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="L20" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="L20" s="8" t="s">
+      <c r="M20" s="8" t="s">
         <v>142</v>
-      </c>
-      <c r="M20" s="8" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="334" thickBot="1">
       <c r="A21" t="s">
+        <v>149</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>151</v>
-      </c>
       <c r="C21" t="s">
+        <v>182</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E21" t="s">
         <v>183</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E21" t="s">
-        <v>184</v>
-      </c>
       <c r="F21" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G21" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="J21" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="H21" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="J21" s="8" t="s">
+      <c r="K21" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="K21" s="8" t="s">
+      <c r="L21" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>162</v>
       </c>
       <c r="M21" s="8"/>
     </row>
     <row r="22" spans="1:13" ht="409.6" thickBot="1">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:13" ht="363" thickBot="1">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G23" s="8"/>
     </row>

</xml_diff>

<commit_message>
add employ proj annual growth and long term growth
</commit_message>
<xml_diff>
--- a/Data/19_dataText/dataText.xlsx
+++ b/Data/19_dataText/dataText.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\19_dataText\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC324C14-B6B2-44DE-9418-F7510B056E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1565F598-EF9E-40C3-A350-99D183F8E37E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -38,12 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="196">
   <si>
-    <t>selfempRate</t>
-  </si>
-  <si>
-    <t>unempRate</t>
-  </si>
-  <si>
     <t>inactiveRate</t>
   </si>
   <si>
@@ -78,9 +72,6 @@
   </si>
   <si>
     <t>starts</t>
-  </si>
-  <si>
-    <t>level3AndAboveRate</t>
   </si>
   <si>
     <t>sustainedPositiveDestinationKS4Rate</t>
@@ -241,15 +232,6 @@
     <t>mapComment</t>
   </si>
   <si>
-    <t>SelfEmployed</t>
-  </si>
-  <si>
-    <t>Unemployed</t>
-  </si>
-  <si>
-    <t>Inactive</t>
-  </si>
-  <si>
     <t>employment rates</t>
   </si>
   <si>
@@ -500,9 +482,6 @@
   </si>
   <si>
     <t>LaComment</t>
-  </si>
-  <si>
-    <t>wfEmployment</t>
   </si>
   <si>
     <t>Growth from 2023 to 2035</t>
@@ -690,6 +669,27 @@
   </si>
   <si>
     <t>inemployment</t>
+  </si>
+  <si>
+    <t>selfemployedRate</t>
+  </si>
+  <si>
+    <t>unemployedRate</t>
+  </si>
+  <si>
+    <t>selfemployed</t>
+  </si>
+  <si>
+    <t>unemployed</t>
+  </si>
+  <si>
+    <t>inactive</t>
+  </si>
+  <si>
+    <t>L3PlusPerc</t>
+  </si>
+  <si>
+    <t>employmentProjection</t>
   </si>
 </sst>
 </file>
@@ -1109,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1122,902 +1122,902 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
       <c r="G1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="I1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="J1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="L1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="M1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="189" thickBot="1">
       <c r="A2" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="189" thickBot="1">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>189</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="189" thickBot="1">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>190</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="189" thickBot="1">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="290.5" thickBot="1">
       <c r="A6" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="189" thickBot="1">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>191</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="189" thickBot="1">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>192</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="189" thickBot="1">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>193</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="203.5" thickBot="1">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="145.5" thickBot="1">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="319.5" thickBot="1">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="319.5" thickBot="1">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="363" thickBot="1">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="363" thickBot="1">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="409.6" thickBot="1">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="409.6" thickBot="1">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="348.5" thickBot="1">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>194</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="263" thickBot="1">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="254" thickBot="1">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="334" thickBot="1">
       <c r="A21" t="s">
-        <v>149</v>
+        <v>195</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C21" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E21" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="M21" s="8"/>
     </row>
     <row r="22" spans="1:13" ht="409.6" thickBot="1">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:13" ht="363" thickBot="1">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="G23" s="8"/>
     </row>

</xml_diff>

<commit_message>
tidy up some file names tidy up libraries add enterprise by industry fix fe subgroups fix business england data add in fe overview charts get breakdowns working
</commit_message>
<xml_diff>
--- a/Data/19_dataText/dataText.xlsx
+++ b/Data/19_dataText/dataText.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\19_dataText\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1565F598-EF9E-40C3-A350-99D183F8E37E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E68F09F-5461-46EA-8B2D-BA8572700C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="195">
   <si>
     <t>inactiveRate</t>
   </si>
@@ -389,9 +389,6 @@
   </si>
   <si>
     <t>FE achievements</t>
-  </si>
-  <si>
-    <t>The FE achievements</t>
   </si>
   <si>
     <t>number of FE achievements</t>
@@ -1109,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1143,30 +1140,30 @@
         <v>58</v>
       </c>
       <c r="H1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I1" t="s">
         <v>137</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>138</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>139</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>140</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>141</v>
-      </c>
-      <c r="M1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="189" thickBot="1">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>27</v>
@@ -1178,13 +1175,13 @@
         <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>40</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>60</v>
@@ -1204,10 +1201,10 @@
     </row>
     <row r="3" spans="1:13" ht="189" thickBot="1">
       <c r="A3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>27</v>
@@ -1219,13 +1216,13 @@
         <v>27</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>41</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>65</v>
@@ -1245,10 +1242,10 @@
     </row>
     <row r="4" spans="1:13" ht="189" thickBot="1">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>27</v>
@@ -1260,13 +1257,13 @@
         <v>27</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>42</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>60</v>
@@ -1289,7 +1286,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>27</v>
@@ -1301,13 +1298,13 @@
         <v>27</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>43</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>72</v>
@@ -1327,10 +1324,10 @@
     </row>
     <row r="6" spans="1:13" ht="290.5" thickBot="1">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>27</v>
@@ -1342,13 +1339,13 @@
         <v>27</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>1</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>76</v>
@@ -1368,10 +1365,10 @@
     </row>
     <row r="7" spans="1:13" ht="189" thickBot="1">
       <c r="A7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>27</v>
@@ -1383,13 +1380,13 @@
         <v>27</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>44</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>80</v>
@@ -1409,10 +1406,10 @@
     </row>
     <row r="8" spans="1:13" ht="189" thickBot="1">
       <c r="A8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>27</v>
@@ -1424,13 +1421,13 @@
         <v>27</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>45</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>84</v>
@@ -1450,10 +1447,10 @@
     </row>
     <row r="9" spans="1:13" ht="189" thickBot="1">
       <c r="A9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>27</v>
@@ -1465,13 +1462,13 @@
         <v>27</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>46</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>88</v>
@@ -1494,7 +1491,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>19</v>
@@ -1506,13 +1503,13 @@
         <v>19</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>47</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>47</v>
@@ -1535,7 +1532,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>28</v>
@@ -1547,13 +1544,13 @@
         <v>28</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>48</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>96</v>
@@ -1576,7 +1573,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>28</v>
@@ -1588,13 +1585,13 @@
         <v>28</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>49</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>101</v>
@@ -1617,7 +1614,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>28</v>
@@ -1629,13 +1626,13 @@
         <v>28</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>50</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>106</v>
@@ -1658,7 +1655,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>32</v>
@@ -1670,13 +1667,13 @@
         <v>18</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>51</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>110</v>
@@ -1685,13 +1682,13 @@
         <v>111</v>
       </c>
       <c r="K14" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="L14" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="M14" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="M14" s="8" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="363" thickBot="1">
@@ -1699,7 +1696,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>33</v>
@@ -1711,28 +1708,28 @@
         <v>18</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>52</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I15" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="L15" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="J15" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="L15" s="8" t="s">
+      <c r="M15" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="409.6" thickBot="1">
@@ -1740,7 +1737,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>38</v>
@@ -1752,28 +1749,28 @@
         <v>18</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>53</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>53</v>
       </c>
       <c r="J16" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="M16" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="M16" s="8" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="409.6" thickBot="1">
@@ -1781,7 +1778,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>39</v>
@@ -1793,36 +1790,36 @@
         <v>18</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>54</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I17" s="8" t="s">
         <v>54</v>
       </c>
       <c r="J17" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="M17" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="M17" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="348.5" thickBot="1">
       <c r="A18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>27</v>
@@ -1834,28 +1831,28 @@
         <v>27</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>55</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>55</v>
       </c>
       <c r="J18" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="L18" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="K18" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="L18" s="8" t="s">
+      <c r="M18" s="8" t="s">
         <v>127</v>
-      </c>
-      <c r="M18" s="8" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="263" thickBot="1">
@@ -1863,7 +1860,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C19" t="s">
         <v>34</v>
@@ -1875,28 +1872,28 @@
         <v>35</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>56</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I19" s="8" t="s">
         <v>56</v>
       </c>
       <c r="J19" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="K19" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="L19" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="L19" s="8" t="s">
+      <c r="M19" s="8" t="s">
         <v>131</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="254" thickBot="1">
@@ -1904,7 +1901,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C20" t="s">
         <v>36</v>
@@ -1916,66 +1913,66 @@
         <v>37</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>57</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>57</v>
       </c>
       <c r="J20" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="K20" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="L20" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="L20" s="8" t="s">
+      <c r="M20" s="8" t="s">
         <v>135</v>
-      </c>
-      <c r="M20" s="8" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="334" thickBot="1">
       <c r="A21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C21" t="s">
+        <v>174</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E21" t="s">
         <v>175</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E21" t="s">
-        <v>176</v>
-      </c>
       <c r="F21" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>76</v>
       </c>
       <c r="J21" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="K21" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="K21" s="8" t="s">
+      <c r="L21" s="8" t="s">
         <v>153</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>154</v>
       </c>
       <c r="M21" s="8"/>
     </row>
@@ -1984,7 +1981,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>31</v>
@@ -1996,7 +1993,7 @@
         <v>18</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G22" s="8"/>
     </row>
@@ -2005,7 +2002,7 @@
         <v>11</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>33</v>
@@ -2017,7 +2014,7 @@
         <v>18</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G23" s="8"/>
     </row>

</xml_diff>

<commit_message>
Add note on skills imperative SOC2020 issue
</commit_message>
<xml_diff>
--- a/Data/19_dataText/dataText.xlsx
+++ b/Data/19_dataText/dataText.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\19_dataText\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hcox\OneDrive - Department for Education\Documents\Projects\Provision mapping\RAG\lsip_dashboard\Data\19_dataText\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27D1717-65AD-4B5C-AA8C-2BAABF20A1D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2E7C0D-0C05-4CD2-B4F4-570A3E654F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
   <sheets>
     <sheet name="dataText" sheetId="1" r:id="rId1"/>
@@ -604,12 +604,6 @@
     <t>will year on year employment volume growth change</t>
   </si>
   <si>
-    <t xml:space="preserve">Projections are from Skills Imperative 2035. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data presented is the baseline projection. Alternative scenarios are available from NFER. </t>
-  </si>
-  <si>
     <t>&lt;ol&gt;
   &lt;li&gt;Figures are for 16-64 year olds.&lt;/li&gt;
 &lt;li&gt;Each estimate from the Annual Population Survey carries a margin of error. These are available in the original data via NOMIS. Large margins of error are usually associated with groups with only a small number of respondents. Therefore, please take caution when interpreting data from small subgroups.&lt;/li&gt;
@@ -676,17 +670,24 @@
 &lt;/ol&gt;</t>
   </si>
   <si>
+    <t>&lt;a href = 'https://www.gov.uk/government/publications/labour-market-and-skills-projections-2020-to-2035'&gt;Skills Imperative 2035&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projections are from Skills Imperative 2035. The occupation projections are based on ONS survey data that has been impacted by a coding error, so should be used with caution.  </t>
+  </si>
+  <si>
+    <t>Data presented is the baseline projection. Alternative scenarios are available from NFER. The occupation projections are based on ONS survey data that has been impacted by a coding error, so should be used with caution.  For more information on the miscoding of occupation data see this  &lt;a href = 'https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/articles/theimpactofmiscodingofoccupationaldatainofficefornationalstatisticssocialsurveysuk/2022-09-26'&gt;ONS article&lt;/a&gt;.</t>
+  </si>
+  <si>
     <t>&lt;ol&gt;
   &lt;li&gt;The projections presented in this Workbook are calculated from a number of different data sources, using a variety of econometric and statistical techniques. As a result, precise margins of error cannot be assigned to the estimates. For further details, see the Technical Report. &lt;/li&gt;
+&lt;li&gt;The occupation projections are based on ONS survey data that has been impacted by a coding error, so should be used with caution.  For more information on the miscoding of occupation data see this  &lt;a href = 'https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/articles/theimpactofmiscodingofoccupationaldatainofficefornationalstatisticssocialsurveysuk/2022-09-26'&gt;ONS article&lt;/a&gt;.&lt;/li&gt;
  &lt;li&gt;Industries are based on SIC 2007 codes. &lt;/li&gt;
  &lt;li&gt;Time series of the breakdowns can be downloaded in the data download section or in the publication. &lt;/li&gt;
  &lt;li&gt;Further breakdowns are available in the published data eg gender, full-time/part-time, as well combined breakdowns. Replacement demand is also available. &lt;/li&gt;
  &lt;li&gt;The projections were largely prepared before the Russian invasion of Ukraine, its subsequent economic effects and policy responses to these events. These factors will have a significant impact on the short-term prospects for the British economy and labour market &lt;/li&gt;
 &lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
 &lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href = 'https://www.gov.uk/government/publications/labour-market-and-skills-projections-2020-to-2035'&gt;Skills Imperative 2035&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -772,23 +773,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1106,917 +1112,917 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="91.06640625" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="25" style="6" customWidth="1"/>
-    <col min="5" max="5" width="32.08984375" customWidth="1"/>
-    <col min="6" max="6" width="51.26953125" customWidth="1"/>
+    <col min="1" max="1" width="91.06640625" style="3"/>
+    <col min="2" max="2" width="91.06640625" style="4"/>
+    <col min="3" max="16384" width="91.06640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" ht="14.65" thickBot="1">
+      <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="189" thickBot="1">
-      <c r="A2" t="s">
+    <row r="2" spans="1:13" ht="114.4" thickBot="1">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="114.4" thickBot="1">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="114.4" thickBot="1">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="114.4" thickBot="1">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="171.4" thickBot="1">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="114.4" thickBot="1">
+      <c r="A7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="114.4" thickBot="1">
+      <c r="A8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="114.4" thickBot="1">
+      <c r="A9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="128.65" thickBot="1">
+      <c r="A10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="189" thickBot="1">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="189" thickBot="1">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="189" thickBot="1">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="290.5" thickBot="1">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="G10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="85.9" thickBot="1">
+      <c r="A11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="189" thickBot="1">
-      <c r="A7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="189" thickBot="1">
-      <c r="A8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="189" thickBot="1">
-      <c r="A9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="203.5" thickBot="1">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="145.5" thickBot="1">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J11" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="L11" s="8" t="s">
+      <c r="L11" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="M11" s="8" t="s">
+      <c r="M11" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="319.5" thickBot="1">
-      <c r="A12" t="s">
+    <row r="12" spans="1:13" ht="185.65" thickBot="1">
+      <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="6" t="s">
         <v>155</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="G12" s="8" t="s">
+      <c r="F12" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="L12" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="M12" s="8" t="s">
+      <c r="M12" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="319.5" thickBot="1">
-      <c r="A13" t="s">
+    <row r="13" spans="1:13" ht="185.65" thickBot="1">
+      <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="6" t="s">
         <v>155</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="G13" s="8" t="s">
+      <c r="F13" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K13" s="8" t="s">
+      <c r="K13" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="L13" s="8" t="s">
+      <c r="L13" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="M13" s="8" t="s">
+      <c r="M13" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="363" thickBot="1">
-      <c r="A14" t="s">
+    <row r="14" spans="1:13" ht="128.65" thickBot="1">
+      <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="G14" s="8" t="s">
+      <c r="F14" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="K14" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="L14" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="M14" s="8" t="s">
+      <c r="M14" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="363" thickBot="1">
-      <c r="A15" t="s">
+    <row r="15" spans="1:13" ht="128.65" thickBot="1">
+      <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>156</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="128.65" thickBot="1">
+      <c r="A16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="128.65" thickBot="1">
+      <c r="A17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="214.15" thickBot="1">
+      <c r="A18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="142.9" thickBot="1">
+      <c r="A19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="G15" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="409.6" thickBot="1">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="6" t="s">
+      <c r="G19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="142.9" thickBot="1">
+      <c r="A20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="271.14999999999998" thickBot="1">
+      <c r="A21" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" ht="128.65" thickBot="1">
+      <c r="A22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="M16" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="409.6" thickBot="1">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="M17" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="348.5" thickBot="1">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="L18" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="M18" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="263" thickBot="1">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="L19" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="254" thickBot="1">
-      <c r="A20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="L20" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="M20" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="334" thickBot="1">
-      <c r="A21" t="s">
-        <v>150</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C21" t="s">
-        <v>183</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E21" t="s">
-        <v>184</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="M21" s="8"/>
-    </row>
-    <row r="22" spans="1:13" ht="409.6" thickBot="1">
-      <c r="A22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="G22" s="8"/>
-    </row>
-    <row r="23" spans="1:13" ht="363" thickBot="1">
-      <c r="A23" t="s">
+      <c r="F22" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" ht="128.65" thickBot="1">
+      <c r="A23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="4" t="s">
         <v>156</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="G23" s="8"/>
+      <c r="F23" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G23" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>